<commit_message>
Update output format for convert_xlsx_to_yaml_calendar
</commit_message>
<xml_diff>
--- a/examples/example_calendar_data.xlsx
+++ b/examples/example_calendar_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25240" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25160" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Week</t>
   </si>
@@ -121,6 +121,108 @@
   </si>
   <si>
     <t>Week 10 Forum Post</t>
+  </si>
+  <si>
+    <t>Readings</t>
+  </si>
+  <si>
+    <t>TB Ch. 1-2|SP1 Ls. 1-3</t>
+  </si>
+  <si>
+    <t>TB Ch. 3-4|SP1 Ls. 4</t>
+  </si>
+  <si>
+    <t>TB Ch. 7-8|SP1 Ls. 5, 11</t>
+  </si>
+  <si>
+    <t>TB Ch. 5-6|SP1 Ls. 6-7</t>
+  </si>
+  <si>
+    <t>TB Ch. 12|SP1 Ls. 10|SP2 Ls. 9</t>
+  </si>
+  <si>
+    <t>TB Ch. 10-11|SP1 Ls. 9|SP2 Ls. 1-2</t>
+  </si>
+  <si>
+    <t>TB Ch. 13|SP2 Ls. 4-5</t>
+  </si>
+  <si>
+    <t>TB Ch. 14-15| SP2 Ls. 7-8</t>
+  </si>
+  <si>
+    <t>TB Ch. 16-17|SP1 Ls. 8|SP2 Ls. 3</t>
+  </si>
+  <si>
+    <t>TB Ch. 19-20|SP2 Ls.  11-12</t>
+  </si>
+  <si>
+    <t>Reading Equivalences</t>
+  </si>
+  <si>
+    <t>Reading Notes</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 1-2 &lt;=&gt; TB Ch. 1|SP1 Ls. 3 &lt;=&gt; TB Ch. 2</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 4 &lt;=&gt; TB Ch. 4</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 6 &lt;=&gt; Ch. 6|SP1 Ls. 7 &lt;=&gt; Ch. 5</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 10 and SP2 Ls. 9 &lt;=&gt; Ch. 12</t>
+  </si>
+  <si>
+    <t>SP2 Ls. 4-5 &lt;=&gt; Ch. 13</t>
+  </si>
+  <si>
+    <t>SP2 Ls. 7 &lt;=&gt; Ch. 14|SP2 Ls. 8 &lt;=&gt; Ch. 15</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 8 &lt;=&gt; Ch. 17|SP2 Ls. 3 &lt;=&gt; Ch. 16</t>
+  </si>
+  <si>
+    <t>SP2 Ls. 11-12 &lt;=&gt; bonus material</t>
+  </si>
+  <si>
+    <t>Review all chapters</t>
+  </si>
+  <si>
+    <t>Chapter 1: SAS programs, libraries, datasets, interface|Chapter 2: libraries, results viewer, global system options</t>
+  </si>
+  <si>
+    <t>Chapter 14: do-loops|Chapter 15: arrays</t>
+  </si>
+  <si>
+    <t>Chapter 16: formatted input in fixed fields|Chapter 17: free-form input</t>
+  </si>
+  <si>
+    <t>Chapter 19: combining observations|Chapter 20: splitting observations</t>
+  </si>
+  <si>
+    <t>Chapter 3: enhanced editor and error messages|Chapter 4: proc print, proc sort, titles, footnotes, formats</t>
+  </si>
+  <si>
+    <t>Chapter 7: proc format|Chapter 8: proc means, proc freq</t>
+  </si>
+  <si>
+    <t>Chapter 5: libraries, raw data files, data step programming, data step variables, subsetting if, _null_ data step, Microsoft Excel import| Chapter 6: data step compilation, execution, &amp; debugging</t>
+  </si>
+  <si>
+    <t>Chapter 12: combining datasets horizontally and vertically</t>
+  </si>
+  <si>
+    <t>Chapter 10: sum notation, retain, if-then-else blocks, length statements, select groups, do groups|Chapter 11: dataset options, by-group processing, point=</t>
+  </si>
+  <si>
+    <t>Chapter 13: data-step functions, where expressions</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 5 &lt;=&gt; TB Ch. 7|SP1 Ls. 11 &lt;=&gt; TB Ch. 8</t>
+  </si>
+  <si>
+    <t>SP1 Ls. 9 and SP2 Ls. 1 &lt;=&gt; Ch. 10|SP2 Ls. 2 &lt;=&gt; Ch. 11</t>
   </si>
 </sst>
 </file>
@@ -169,7 +271,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -223,11 +325,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -254,6 +364,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -280,6 +391,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,176 +721,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="45">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+    <row r="3" spans="1:7" ht="45">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="75">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="60">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="30">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update file format for convert_xlsx_to_yaml_calendar
</commit_message>
<xml_diff>
--- a/examples/example_calendar_data.xlsx
+++ b/examples/example_calendar_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25160" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="24600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -156,12 +156,6 @@
     <t>TB Ch. 19-20|SP2 Ls.  11-12</t>
   </si>
   <si>
-    <t>Reading Equivalences</t>
-  </si>
-  <si>
-    <t>Reading Notes</t>
-  </si>
-  <si>
     <t>SP1 Ls. 1-2 &lt;=&gt; TB Ch. 1|SP1 Ls. 3 &lt;=&gt; TB Ch. 2</t>
   </si>
   <si>
@@ -223,6 +217,12 @@
   </si>
   <si>
     <t>SP1 Ls. 9 and SP2 Ls. 1 &lt;=&gt; Ch. 10|SP2 Ls. 2 &lt;=&gt; Ch. 11</t>
+  </si>
+  <si>
+    <t>Reading_Notes</t>
+  </si>
+  <si>
+    <t>Reading_Equivalences</t>
   </si>
 </sst>
 </file>
@@ -744,10 +744,10 @@
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -767,10 +767,10 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
@@ -788,10 +788,10 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
@@ -811,10 +811,10 @@
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>17</v>
@@ -834,10 +834,10 @@
         <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
@@ -857,10 +857,10 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
@@ -880,10 +880,10 @@
         <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
@@ -903,10 +903,10 @@
         <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>21</v>
@@ -926,10 +926,10 @@
         <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
@@ -949,10 +949,10 @@
         <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
@@ -972,10 +972,10 @@
         <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
@@ -992,7 +992,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>

</xml_diff>

<commit_message>
Update example data, including using Excel formulas
</commit_message>
<xml_diff>
--- a/examples/example_calendar_data.xlsx
+++ b/examples/example_calendar_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Week</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Week 1 Setup|Week 1 Reflections</t>
-  </si>
-  <si>
     <t>Project 1 Step 1 Final</t>
   </si>
   <si>
@@ -63,63 +60,6 @@
     <t>Project 2 Code Review|Final Exam</t>
   </si>
   <si>
-    <t>Week 2 Reflection</t>
-  </si>
-  <si>
-    <t>Week 1 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 3 Reflection</t>
-  </si>
-  <si>
-    <t>Week 4 Reflection</t>
-  </si>
-  <si>
-    <t>Week 5 Reflection</t>
-  </si>
-  <si>
-    <t>Week 6 Reflection</t>
-  </si>
-  <si>
-    <t>Week 7 Reflection</t>
-  </si>
-  <si>
-    <t>Week 8 Reflection</t>
-  </si>
-  <si>
-    <t>Week 9 Reflection</t>
-  </si>
-  <si>
-    <t>Week 10 Reflection</t>
-  </si>
-  <si>
-    <t>Week 2 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 3 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 4 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 5 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 6 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 7 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 8 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 9 Forum Post</t>
-  </si>
-  <si>
-    <t>Week 10 Forum Post</t>
-  </si>
-  <si>
     <t>Readings</t>
   </si>
   <si>
@@ -223,6 +163,9 @@
   </si>
   <si>
     <t>Review all|chapters</t>
+  </si>
+  <si>
+    <t>Week 1 Setup|Week 1 Quiz</t>
   </si>
 </sst>
 </file>
@@ -271,8 +214,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,7 +288,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -371,6 +318,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -400,6 +349,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,7 +682,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -739,9 +695,9 @@
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -749,13 +705,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -772,20 +728,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
+      <c r="F2" s="1" t="str">
+        <f>"Week "&amp;$A2&amp;" Forum Post"</f>
+        <v>Week 1 Forum Post</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45">
@@ -793,22 +750,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>"Week "&amp;$A3&amp;" Quiz"</f>
+        <v>Week 2 Quiz</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F11" si="0">"Week "&amp;$A3&amp;" Forum Post"</f>
+        <v>Week 2 Forum Post</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30">
@@ -816,22 +775,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E11" si="1">"Week "&amp;$A4&amp;" Quiz"</f>
+        <v>Week 3 Quiz</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 3 Forum Post</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75">
@@ -839,22 +800,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 4 Quiz</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 4 Forum Post</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30">
@@ -862,22 +825,24 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 5 Quiz</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 5 Forum Post</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60">
@@ -885,22 +850,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 6 Quiz</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 6 Forum Post</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
@@ -908,22 +875,24 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 7 Quiz</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 7 Forum Post</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -931,22 +900,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 8 Quiz</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 8 Forum Post</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30">
@@ -954,22 +925,24 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 9 Quiz</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 9 Forum Post</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
@@ -977,22 +950,24 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Week 10 Quiz</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Week 10 Forum Post</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1000,14 +975,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>